<commit_message>
Usuarios y contraseñas de dispositivos
</commit_message>
<xml_diff>
--- a/Diseño/ProyectoRedes.xlsx
+++ b/Diseño/ProyectoRedes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldo_\Documents\PROYECTO REDES\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E53472-BA7F-45A3-8B24-AF48FA3EA756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309592A8-8B03-4C09-8CF3-826485AC1238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{53B3A9C0-512B-4520-BD87-E071D9525003}"/>
   </bookViews>
@@ -2099,7 +2099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2404,9 +2404,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2416,24 +2434,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2445,27 +2445,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2852,7 +2831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0819F73E-3536-4D34-9E0B-51FD655C1870}">
   <dimension ref="A2:Y152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="T62" sqref="T62"/>
     </sheetView>
   </sheetViews>
@@ -2866,46 +2845,46 @@
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="10" width="20.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
     <col min="18" max="18" width="14.140625" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
     <col min="21" max="21" width="12.5703125" customWidth="1"/>
     <col min="22" max="22" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="111" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
     </row>
     <row r="3" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
     </row>
     <row r="4" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="113"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2920,10 +2899,10 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="115"/>
+      <c r="C6" s="121"/>
       <c r="D6" s="2">
         <f>80+82+80</f>
         <v>242</v>
@@ -3163,8 +3142,8 @@
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
     </row>
     <row r="18" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
@@ -3328,65 +3307,65 @@
     </row>
     <row r="28" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="17"/>
-      <c r="J28" s="117" t="s">
+      <c r="J28" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="K28" s="117"/>
-      <c r="L28" s="117"/>
-      <c r="M28" s="117"/>
-      <c r="N28" s="117"/>
-      <c r="O28" s="117"/>
-      <c r="P28" s="117"/>
+      <c r="K28" s="113"/>
+      <c r="L28" s="113"/>
+      <c r="M28" s="113"/>
+      <c r="N28" s="113"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="113"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="18"/>
-      <c r="S28" s="118" t="s">
+      <c r="S28" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="T28" s="119"/>
+      <c r="T28" s="116"/>
     </row>
     <row r="29" spans="2:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="117" t="s">
+      <c r="B29" s="113" t="s">
         <v>152</v>
       </c>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
-      <c r="E29" s="117"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
       <c r="I29" s="17"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="117"/>
-      <c r="L29" s="117"/>
-      <c r="M29" s="117"/>
-      <c r="N29" s="117"/>
-      <c r="O29" s="117"/>
-      <c r="P29" s="117"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="113"/>
+      <c r="L29" s="113"/>
+      <c r="M29" s="113"/>
+      <c r="N29" s="113"/>
+      <c r="O29" s="113"/>
+      <c r="P29" s="113"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="19"/>
-      <c r="S29" s="120" t="s">
+      <c r="S29" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="T29" s="121"/>
+      <c r="T29" s="118"/>
       <c r="U29" s="16"/>
       <c r="V29" s="16"/>
     </row>
     <row r="30" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
-      <c r="E30" s="117"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
       <c r="I30" s="17"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="117"/>
-      <c r="L30" s="117"/>
-      <c r="M30" s="117"/>
-      <c r="N30" s="117"/>
-      <c r="O30" s="117"/>
-      <c r="P30" s="117"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="113"/>
+      <c r="L30" s="113"/>
+      <c r="M30" s="113"/>
+      <c r="N30" s="113"/>
+      <c r="O30" s="113"/>
+      <c r="P30" s="113"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="22"/>
-      <c r="S30" s="120" t="s">
+      <c r="S30" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="T30" s="121"/>
+      <c r="T30" s="118"/>
       <c r="U30" s="16"/>
       <c r="V30" s="16"/>
     </row>
@@ -3407,28 +3386,28 @@
       <c r="G32" s="63" t="s">
         <v>407</v>
       </c>
-      <c r="J32" s="127" t="s">
+      <c r="J32" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="K32" s="127" t="s">
+      <c r="K32" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="L32" s="127" t="s">
+      <c r="L32" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="M32" s="127" t="s">
+      <c r="M32" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="N32" s="127" t="s">
+      <c r="N32" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="O32" s="127" t="s">
+      <c r="O32" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="P32" s="127" t="s">
+      <c r="P32" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="Q32" s="127" t="s">
+      <c r="Q32" s="66" t="s">
         <v>74</v>
       </c>
       <c r="R32" s="66" t="s">
@@ -3437,13 +3416,13 @@
       <c r="S32" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="T32" s="127" t="s">
+      <c r="T32" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="U32" s="127" t="s">
+      <c r="U32" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="V32" s="132" t="s">
+      <c r="V32" s="23" t="s">
         <v>148</v>
       </c>
       <c r="W32" s="66" t="s">
@@ -3473,7 +3452,7 @@
         <v>397</v>
       </c>
       <c r="H33" s="15"/>
-      <c r="I33" s="127" t="s">
+      <c r="I33" s="66" t="s">
         <v>145</v>
       </c>
       <c r="J33" s="21"/>
@@ -3510,7 +3489,7 @@
         <v>398</v>
       </c>
       <c r="H34" s="15"/>
-      <c r="I34" s="127" t="s">
+      <c r="I34" s="66" t="s">
         <v>71</v>
       </c>
       <c r="J34" s="18"/>
@@ -3547,7 +3526,7 @@
         <v>403</v>
       </c>
       <c r="H35" s="15"/>
-      <c r="I35" s="127" t="s">
+      <c r="I35" s="66" t="s">
         <v>72</v>
       </c>
       <c r="J35" s="18"/>
@@ -3584,7 +3563,7 @@
         <v>395</v>
       </c>
       <c r="H36" s="15"/>
-      <c r="I36" s="127" t="s">
+      <c r="I36" s="66" t="s">
         <v>76</v>
       </c>
       <c r="J36" s="18"/>
@@ -3621,7 +3600,7 @@
         <v>400</v>
       </c>
       <c r="H37" s="15"/>
-      <c r="I37" s="127" t="s">
+      <c r="I37" s="66" t="s">
         <v>73</v>
       </c>
       <c r="J37" s="18"/>
@@ -3658,7 +3637,7 @@
         <v>406</v>
       </c>
       <c r="H38" s="15"/>
-      <c r="I38" s="131" t="s">
+      <c r="I38" s="59" t="s">
         <v>77</v>
       </c>
       <c r="J38" s="18"/>
@@ -3695,7 +3674,7 @@
         <v>405</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="127" t="s">
+      <c r="I39" s="66" t="s">
         <v>78</v>
       </c>
       <c r="J39" s="18"/>
@@ -3719,10 +3698,10 @@
       <c r="B40" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="127" t="s">
+      <c r="C40" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="128" t="s">
+      <c r="D40" s="62" t="s">
         <v>94</v>
       </c>
       <c r="E40" s="62">
@@ -3732,7 +3711,7 @@
         <v>392</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="131" t="s">
+      <c r="I40" s="59" t="s">
         <v>74</v>
       </c>
       <c r="J40" s="18"/>
@@ -3756,10 +3735,10 @@
       <c r="B41" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="127" t="s">
+      <c r="C41" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="128" t="s">
+      <c r="D41" s="62" t="s">
         <v>147</v>
       </c>
       <c r="E41" s="62">
@@ -3769,7 +3748,7 @@
         <v>402</v>
       </c>
       <c r="H41" s="15"/>
-      <c r="I41" s="127" t="s">
+      <c r="I41" s="66" t="s">
         <v>79</v>
       </c>
       <c r="J41" s="18"/>
@@ -3796,10 +3775,10 @@
       <c r="B42" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="129" t="s">
+      <c r="C42" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="128" t="s">
+      <c r="D42" s="62" t="s">
         <v>149</v>
       </c>
       <c r="E42" s="62">
@@ -3833,10 +3812,10 @@
       <c r="B43" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="C43" s="129" t="s">
+      <c r="C43" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="129" t="s">
+      <c r="D43" s="23" t="s">
         <v>178</v>
       </c>
       <c r="E43" s="23">
@@ -3844,7 +3823,7 @@
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="131" t="s">
+      <c r="I43" s="59" t="s">
         <v>75</v>
       </c>
       <c r="J43" s="18"/>
@@ -3868,10 +3847,10 @@
       <c r="B44" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="127" t="s">
+      <c r="C44" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="128" t="s">
+      <c r="D44" s="62" t="s">
         <v>96</v>
       </c>
       <c r="E44" s="62">
@@ -3881,7 +3860,7 @@
         <v>393</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="127" t="s">
+      <c r="I44" s="66" t="s">
         <v>80</v>
       </c>
       <c r="J44" s="18"/>
@@ -3905,10 +3884,10 @@
       <c r="B45" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="127" t="s">
+      <c r="C45" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="128" t="s">
+      <c r="D45" s="62" t="s">
         <v>98</v>
       </c>
       <c r="E45" s="62">
@@ -3918,7 +3897,7 @@
         <v>394</v>
       </c>
       <c r="H45" s="15"/>
-      <c r="I45" s="132" t="s">
+      <c r="I45" s="23" t="s">
         <v>148</v>
       </c>
       <c r="J45" s="18"/>
@@ -3942,10 +3921,10 @@
       <c r="B46" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="127" t="s">
+      <c r="C46" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="128" t="s">
+      <c r="D46" s="62" t="s">
         <v>103</v>
       </c>
       <c r="E46" s="62">
@@ -3979,10 +3958,10 @@
       <c r="B47" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="C47" s="127" t="s">
+      <c r="C47" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="130" t="s">
+      <c r="D47" s="61" t="s">
         <v>146</v>
       </c>
       <c r="E47" s="62">
@@ -4070,8 +4049,8 @@
       <c r="F54" s="111"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114"/>
       <c r="H55" s="15"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.25">
@@ -4868,8 +4847,8 @@
       <c r="L75" s="25"/>
     </row>
     <row r="76" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E76" s="112"/>
-      <c r="F76" s="112"/>
+      <c r="E76" s="114"/>
+      <c r="F76" s="114"/>
       <c r="H76" s="15"/>
       <c r="I76" s="25"/>
       <c r="K76" s="24"/>
@@ -5258,8 +5237,8 @@
       <c r="F95" s="111"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E96" s="112"/>
-      <c r="F96" s="112"/>
+      <c r="E96" s="114"/>
+      <c r="F96" s="114"/>
       <c r="H96" s="15"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -5637,8 +5616,8 @@
       <c r="F115" s="111"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E116" s="112"/>
-      <c r="F116" s="112"/>
+      <c r="E116" s="114"/>
+      <c r="F116" s="114"/>
       <c r="H116" s="15"/>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.25">
@@ -6016,8 +5995,8 @@
       <c r="F135" s="111"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E136" s="112"/>
-      <c r="F136" s="112"/>
+      <c r="E136" s="114"/>
+      <c r="F136" s="114"/>
       <c r="H136" s="15"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
@@ -6395,6 +6374,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="E95:F96"/>
+    <mergeCell ref="E115:F116"/>
+    <mergeCell ref="E135:F136"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="J28:P30"/>
     <mergeCell ref="E75:F76"/>
@@ -6403,11 +6387,6 @@
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="E54:F55"/>
     <mergeCell ref="B29:E30"/>
-    <mergeCell ref="E95:F96"/>
-    <mergeCell ref="E115:F116"/>
-    <mergeCell ref="E135:F136"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6454,33 +6433,33 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="J4" s="117" t="s">
+      <c r="J4" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
       <c r="S4" s="18"/>
-      <c r="T4" s="118" t="s">
+      <c r="T4" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="U4" s="119"/>
+      <c r="U4" s="116"/>
     </row>
     <row r="5" spans="3:42" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="113"/>
+      <c r="O5" s="113"/>
+      <c r="P5" s="113"/>
+      <c r="Q5" s="113"/>
+      <c r="R5" s="113"/>
       <c r="S5" s="19"/>
       <c r="T5" s="122" t="s">
         <v>84</v>
@@ -6490,15 +6469,15 @@
       <c r="W5" s="16"/>
     </row>
     <row r="6" spans="3:42" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="113"/>
+      <c r="N6" s="113"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="113"/>
+      <c r="Q6" s="113"/>
+      <c r="R6" s="113"/>
       <c r="S6" s="22"/>
       <c r="T6" s="122" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Mascaras corregidas de todos los nodos
</commit_message>
<xml_diff>
--- a/Diseño/ProyectoRedes.xlsx
+++ b/Diseño/ProyectoRedes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldo_\Documents\PROYECTO REDES\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D75161-6A8F-4AA0-A069-56A097AB9277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B2473E-B3F2-4AAF-9AEA-BBF04A6A7F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{53B3A9C0-512B-4520-BD87-E071D9525003}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{53B3A9C0-512B-4520-BD87-E071D9525003}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECCIONAMIENTO_GPP" sheetId="1" r:id="rId1"/>
@@ -2620,7 +2620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2831,12 +2831,55 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2846,62 +2889,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3233,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0819F73E-3536-4D34-9E0B-51FD655C1870}">
   <dimension ref="A2:Y152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,29 +3256,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="78"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3301,10 +3293,10 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="80"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="2">
         <f>80+82+80</f>
         <v>242</v>
@@ -3709,65 +3701,65 @@
     </row>
     <row r="28" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="17"/>
-      <c r="J28" s="82" t="s">
+      <c r="J28" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="82"/>
-      <c r="L28" s="82"/>
-      <c r="M28" s="82"/>
-      <c r="N28" s="82"/>
-      <c r="O28" s="82"/>
-      <c r="P28" s="82"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="87"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="18"/>
-      <c r="S28" s="83" t="s">
+      <c r="S28" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="T28" s="84"/>
+      <c r="T28" s="90"/>
     </row>
     <row r="29" spans="2:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
       <c r="I29" s="17"/>
-      <c r="J29" s="82"/>
-      <c r="K29" s="82"/>
-      <c r="L29" s="82"/>
-      <c r="M29" s="82"/>
-      <c r="N29" s="82"/>
-      <c r="O29" s="82"/>
-      <c r="P29" s="82"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="87"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="19"/>
-      <c r="S29" s="85" t="s">
+      <c r="S29" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="T29" s="86"/>
+      <c r="T29" s="92"/>
       <c r="U29" s="16"/>
       <c r="V29" s="16"/>
     </row>
     <row r="30" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
       <c r="I30" s="17"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="82"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="82"/>
-      <c r="O30" s="82"/>
-      <c r="P30" s="82"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="87"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="22"/>
-      <c r="S30" s="85" t="s">
+      <c r="S30" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="T30" s="86"/>
+      <c r="T30" s="92"/>
       <c r="U30" s="16"/>
       <c r="V30" s="16"/>
     </row>
@@ -4445,14 +4437,14 @@
       <c r="B52" s="28"/>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E54" s="76" t="s">
+      <c r="E54" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="F54" s="76"/>
+      <c r="F54" s="85"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E55" s="77"/>
-      <c r="F55" s="77"/>
+      <c r="E55" s="88"/>
+      <c r="F55" s="88"/>
       <c r="H55" s="15"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.25">
@@ -5240,16 +5232,16 @@
       <c r="L74" s="25"/>
     </row>
     <row r="75" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E75" s="76" t="s">
+      <c r="E75" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="F75" s="76"/>
+      <c r="F75" s="85"/>
       <c r="K75" s="24"/>
       <c r="L75" s="25"/>
     </row>
     <row r="76" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E76" s="77"/>
-      <c r="F76" s="77"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="88"/>
       <c r="H76" s="15"/>
       <c r="I76" s="25"/>
       <c r="K76" s="24"/>
@@ -5632,14 +5624,14 @@
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E95" s="76" t="s">
+      <c r="E95" s="85" t="s">
         <v>240</v>
       </c>
-      <c r="F95" s="76"/>
+      <c r="F95" s="85"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E96" s="77"/>
-      <c r="F96" s="77"/>
+      <c r="E96" s="88"/>
+      <c r="F96" s="88"/>
       <c r="H96" s="15"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -6011,14 +6003,14 @@
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E115" s="76" t="s">
+      <c r="E115" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="F115" s="76"/>
+      <c r="F115" s="85"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E116" s="77"/>
-      <c r="F116" s="77"/>
+      <c r="E116" s="88"/>
+      <c r="F116" s="88"/>
       <c r="H116" s="15"/>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.25">
@@ -6390,14 +6382,14 @@
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E135" s="76" t="s">
+      <c r="E135" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="F135" s="76"/>
+      <c r="F135" s="85"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E136" s="77"/>
-      <c r="F136" s="77"/>
+      <c r="E136" s="88"/>
+      <c r="F136" s="88"/>
       <c r="H136" s="15"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
@@ -6775,6 +6767,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="E95:F96"/>
+    <mergeCell ref="E115:F116"/>
+    <mergeCell ref="E135:F136"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="J28:P30"/>
     <mergeCell ref="E75:F76"/>
@@ -6783,11 +6780,6 @@
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="E54:F55"/>
     <mergeCell ref="B29:E30"/>
-    <mergeCell ref="E95:F96"/>
-    <mergeCell ref="E115:F116"/>
-    <mergeCell ref="E135:F136"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6819,18 +6811,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="96" t="s">
         <v>517</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C3" s="13" t="s">
@@ -6915,9 +6907,6 @@
       <c r="F8" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G8" s="97"/>
-      <c r="H8" s="97"/>
-      <c r="I8" s="87"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
@@ -6947,9 +6936,6 @@
       <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
       <c r="K9" s="36"/>
     </row>
     <row r="10" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6965,9 +6951,6 @@
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
       <c r="K10" s="36"/>
     </row>
     <row r="11" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6983,9 +6966,6 @@
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
       <c r="K11" s="36"/>
     </row>
     <row r="12" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7001,9 +6981,6 @@
       <c r="F12" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7019,9 +6996,6 @@
       <c r="F13" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
       <c r="K13" s="36"/>
     </row>
     <row r="14" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7037,9 +7011,6 @@
       <c r="F14" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
       <c r="K14" s="27"/>
     </row>
     <row r="15" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7055,9 +7026,6 @@
       <c r="F15" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
       <c r="K15" s="36"/>
     </row>
     <row r="16" spans="3:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7073,9 +7041,6 @@
       <c r="F16" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
       <c r="K16" s="27"/>
     </row>
     <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7091,9 +7056,6 @@
       <c r="F17" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
       <c r="K17" s="36"/>
     </row>
     <row r="18" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7109,9 +7071,6 @@
       <c r="F18" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
       <c r="K18" s="36"/>
     </row>
     <row r="19" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7127,9 +7086,6 @@
       <c r="F19" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
       <c r="K19" s="27"/>
     </row>
     <row r="20" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7145,9 +7101,6 @@
       <c r="F20" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G20" s="87"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
       <c r="K20" s="36"/>
     </row>
     <row r="21" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7163,9 +7116,6 @@
       <c r="F21" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
       <c r="K21" s="37"/>
     </row>
     <row r="22" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7181,9 +7131,6 @@
       <c r="F22" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
       <c r="K22" s="36"/>
     </row>
     <row r="23" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7199,298 +7146,195 @@
       <c r="F23" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
       <c r="K23" s="36"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="87"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="87"/>
-    </row>
     <row r="33" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="89"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
     </row>
     <row r="34" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="89"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
     </row>
     <row r="35" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
     </row>
     <row r="36" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="88"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
     </row>
     <row r="37" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C37" s="88"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="90"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="89"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="77"/>
     </row>
     <row r="38" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="88"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="77"/>
     </row>
     <row r="39" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
     </row>
     <row r="40" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C40" s="88"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="88"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="90"/>
-      <c r="H40" s="89"/>
-      <c r="I40" s="89"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="77"/>
     </row>
     <row r="41" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C41" s="88"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="88"/>
-      <c r="F41" s="88"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="89"/>
-      <c r="I41" s="89"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="77"/>
     </row>
     <row r="42" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="89"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="77"/>
     </row>
     <row r="43" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C43" s="88"/>
-      <c r="D43" s="88"/>
-      <c r="E43" s="88"/>
-      <c r="F43" s="88"/>
-      <c r="G43" s="90"/>
-      <c r="H43" s="89"/>
-      <c r="I43" s="89"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
     </row>
     <row r="44" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C44" s="88"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="88"/>
-      <c r="F44" s="88"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
     </row>
     <row r="45" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="77"/>
     </row>
     <row r="46" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C46" s="88"/>
-      <c r="D46" s="88"/>
-      <c r="E46" s="88"/>
-      <c r="F46" s="88"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="89"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="77"/>
     </row>
     <row r="47" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="88"/>
-      <c r="F47" s="88"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="89"/>
-      <c r="I47" s="89"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
     </row>
     <row r="48" spans="3:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="91"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="89"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
     </row>
     <row r="49" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
-      <c r="E49" s="92"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="77"/>
     </row>
     <row r="50" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C50" s="94"/>
-      <c r="D50" s="94"/>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="89"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="79"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="77"/>
     </row>
     <row r="51" spans="3:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C51" s="87"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="95"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="89"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="77"/>
     </row>
     <row r="52" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C52" s="87"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="89"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="77"/>
     </row>
     <row r="53" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C53" s="87"/>
-      <c r="D53" s="87"/>
-      <c r="E53" s="90"/>
-      <c r="F53" s="90"/>
-      <c r="G53" s="87"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="89"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="77"/>
     </row>
     <row r="54" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C54" s="87"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="87"/>
-      <c r="F54" s="90"/>
-      <c r="G54" s="87"/>
-      <c r="H54" s="96"/>
-      <c r="I54" s="96"/>
+      <c r="F54" s="15"/>
+      <c r="H54" s="82"/>
+      <c r="I54" s="82"/>
     </row>
     <row r="55" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C55" s="87"/>
-      <c r="D55" s="87"/>
-      <c r="E55" s="87"/>
-      <c r="F55" s="90"/>
-      <c r="G55" s="87"/>
-      <c r="H55" s="89"/>
-      <c r="I55" s="89"/>
+      <c r="F55" s="15"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F56" s="15"/>
@@ -7528,20 +7372,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="96" t="s">
         <v>727</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="13" t="s">
@@ -7565,1089 +7409,1089 @@
       <c r="I3" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="J3" s="100"/>
+      <c r="J3" s="83"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="84" t="s">
         <v>525</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="84" t="s">
         <v>526</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="84" t="s">
         <v>527</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="84" t="s">
         <v>528</v>
       </c>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101" t="s">
+      <c r="G4" s="84"/>
+      <c r="H4" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="I4" s="101" t="s">
+      <c r="I4" s="84" t="s">
         <v>530</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="83"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="84" t="s">
         <v>531</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="84" t="s">
         <v>532</v>
       </c>
-      <c r="E5" s="101" t="s">
+      <c r="E5" s="84" t="s">
         <v>533</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="84" t="s">
         <v>534</v>
       </c>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101" t="s">
+      <c r="G5" s="84"/>
+      <c r="H5" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="I5" s="101" t="s">
+      <c r="I5" s="84" t="s">
         <v>535</v>
       </c>
-      <c r="J5" s="100"/>
+      <c r="J5" s="83"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="84" t="s">
         <v>536</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="84" t="s">
         <v>537</v>
       </c>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="84" t="s">
         <v>538</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101" t="s">
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="I6" s="101" t="s">
+      <c r="I6" s="84" t="s">
         <v>539</v>
       </c>
-      <c r="J6" s="100"/>
+      <c r="J6" s="83"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="84" t="s">
         <v>541</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="84" t="s">
         <v>542</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101" t="s">
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="I7" s="101" t="s">
+      <c r="I7" s="84" t="s">
         <v>543</v>
       </c>
-      <c r="J7" s="100"/>
+      <c r="J7" s="83"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="84" t="s">
         <v>544</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="84" t="s">
         <v>545</v>
       </c>
-      <c r="E8" s="101" t="s">
+      <c r="E8" s="84" t="s">
         <v>546</v>
       </c>
-      <c r="F8" s="101" t="s">
+      <c r="F8" s="84" t="s">
         <v>547</v>
       </c>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101" t="s">
+      <c r="G8" s="84"/>
+      <c r="H8" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I8" s="101" t="s">
+      <c r="I8" s="84" t="s">
         <v>549</v>
       </c>
-      <c r="J8" s="100"/>
+      <c r="J8" s="83"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="84" t="s">
         <v>550</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="84" t="s">
         <v>551</v>
       </c>
-      <c r="E9" s="101" t="s">
+      <c r="E9" s="84" t="s">
         <v>552</v>
       </c>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="84" t="s">
         <v>553</v>
       </c>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101" t="s">
+      <c r="G9" s="84"/>
+      <c r="H9" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I9" s="101" t="s">
+      <c r="I9" s="84" t="s">
         <v>554</v>
       </c>
-      <c r="J9" s="100"/>
+      <c r="J9" s="83"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="101" t="s">
+      <c r="C10" s="84" t="s">
         <v>555</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="84" t="s">
         <v>556</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="84" t="s">
         <v>528</v>
       </c>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="84" t="s">
         <v>557</v>
       </c>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101" t="s">
+      <c r="G10" s="84"/>
+      <c r="H10" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I10" s="101" t="s">
+      <c r="I10" s="84" t="s">
         <v>558</v>
       </c>
-      <c r="J10" s="100"/>
+      <c r="J10" s="83"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="84" t="s">
         <v>559</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="84" t="s">
         <v>560</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="84" t="s">
         <v>561</v>
       </c>
-      <c r="F11" s="101" t="s">
+      <c r="F11" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101" t="s">
+      <c r="G11" s="84"/>
+      <c r="H11" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I11" s="101" t="s">
+      <c r="I11" s="84" t="s">
         <v>563</v>
       </c>
-      <c r="J11" s="100"/>
+      <c r="J11" s="83"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="84" t="s">
         <v>564</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="84" t="s">
         <v>565</v>
       </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101" t="s">
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I12" s="101" t="s">
+      <c r="I12" s="84" t="s">
         <v>566</v>
       </c>
-      <c r="J12" s="100"/>
+      <c r="J12" s="83"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="84" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="84" t="s">
         <v>568</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="84" t="s">
         <v>569</v>
       </c>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101" t="s">
+      <c r="G13" s="84"/>
+      <c r="H13" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I13" s="101" t="s">
+      <c r="I13" s="84" t="s">
         <v>570</v>
       </c>
-      <c r="J13" s="100"/>
+      <c r="J13" s="83"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="84" t="s">
         <v>571</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="84" t="s">
         <v>572</v>
       </c>
-      <c r="E14" s="101" t="s">
+      <c r="E14" s="84" t="s">
         <v>573</v>
       </c>
-      <c r="F14" s="101" t="s">
+      <c r="F14" s="84" t="s">
         <v>574</v>
       </c>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101" t="s">
+      <c r="G14" s="84"/>
+      <c r="H14" s="84" t="s">
         <v>548</v>
       </c>
-      <c r="I14" s="101" t="s">
+      <c r="I14" s="84" t="s">
         <v>575</v>
       </c>
-      <c r="J14" s="100"/>
+      <c r="J14" s="83"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="84" t="s">
         <v>576</v>
       </c>
-      <c r="D15" s="101" t="s">
+      <c r="D15" s="84" t="s">
         <v>577</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="84" t="s">
         <v>578</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101" t="s">
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="101" t="s">
+      <c r="I15" s="84" t="s">
         <v>579</v>
       </c>
-      <c r="J15" s="100"/>
+      <c r="J15" s="83"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="84" t="s">
         <v>536</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="D16" s="84" t="s">
         <v>580</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="84" t="s">
         <v>581</v>
       </c>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101" t="s">
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="I16" s="101" t="s">
+      <c r="I16" s="84" t="s">
         <v>582</v>
       </c>
-      <c r="J16" s="100"/>
+      <c r="J16" s="83"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="84" t="s">
         <v>583</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="D17" s="84" t="s">
         <v>584</v>
       </c>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="84" t="s">
         <v>527</v>
       </c>
-      <c r="F17" s="101" t="s">
+      <c r="F17" s="84" t="s">
         <v>585</v>
       </c>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101" t="s">
+      <c r="G17" s="84"/>
+      <c r="H17" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="101" t="s">
+      <c r="I17" s="84" t="s">
         <v>586</v>
       </c>
-      <c r="J17" s="100"/>
+      <c r="J17" s="83"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="84" t="s">
         <v>587</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="84" t="s">
         <v>589</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="84" t="s">
         <v>590</v>
       </c>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101" t="s">
+      <c r="G18" s="84"/>
+      <c r="H18" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="101" t="s">
+      <c r="I18" s="84" t="s">
         <v>591</v>
       </c>
-      <c r="J18" s="100"/>
+      <c r="J18" s="83"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="101" t="s">
+      <c r="C19" s="84" t="s">
         <v>592</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="84" t="s">
         <v>593</v>
       </c>
-      <c r="E19" s="101" t="s">
+      <c r="E19" s="84" t="s">
         <v>594</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="84" t="s">
         <v>595</v>
       </c>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101" t="s">
+      <c r="G19" s="84"/>
+      <c r="H19" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="101" t="s">
+      <c r="I19" s="84" t="s">
         <v>596</v>
       </c>
-      <c r="J19" s="100"/>
+      <c r="J19" s="83"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="84" t="s">
         <v>597</v>
       </c>
-      <c r="D20" s="101" t="s">
+      <c r="D20" s="84" t="s">
         <v>598</v>
       </c>
-      <c r="E20" s="101" t="s">
+      <c r="E20" s="84" t="s">
         <v>599</v>
       </c>
-      <c r="F20" s="101" t="s">
+      <c r="F20" s="84" t="s">
         <v>600</v>
       </c>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101" t="s">
+      <c r="G20" s="84"/>
+      <c r="H20" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="101" t="s">
+      <c r="I20" s="84" t="s">
         <v>601</v>
       </c>
-      <c r="J20" s="100"/>
+      <c r="J20" s="83"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="84" t="s">
         <v>602</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="84" t="s">
         <v>597</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="84" t="s">
         <v>603</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="84" t="s">
         <v>604</v>
       </c>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101" t="s">
+      <c r="G21" s="84"/>
+      <c r="H21" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="I21" s="101" t="s">
+      <c r="I21" s="84" t="s">
         <v>605</v>
       </c>
-      <c r="J21" s="100"/>
+      <c r="J21" s="83"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="84" t="s">
         <v>606</v>
       </c>
-      <c r="D22" s="101" t="s">
+      <c r="D22" s="84" t="s">
         <v>607</v>
       </c>
-      <c r="E22" s="101" t="s">
+      <c r="E22" s="84" t="s">
         <v>569</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101" t="s">
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="101" t="s">
+      <c r="I22" s="84" t="s">
         <v>608</v>
       </c>
-      <c r="J22" s="100"/>
+      <c r="J22" s="83"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="84" t="s">
         <v>609</v>
       </c>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="84" t="s">
         <v>610</v>
       </c>
-      <c r="E23" s="101" t="s">
+      <c r="E23" s="84" t="s">
         <v>611</v>
       </c>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101" t="s">
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="I23" s="101" t="s">
+      <c r="I23" s="84" t="s">
         <v>612</v>
       </c>
-      <c r="J23" s="100"/>
+      <c r="J23" s="83"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="84" t="s">
         <v>613</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="84" t="s">
         <v>614</v>
       </c>
-      <c r="E24" s="101" t="s">
+      <c r="E24" s="84" t="s">
         <v>604</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="84" t="s">
         <v>581</v>
       </c>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101" t="s">
+      <c r="G24" s="84"/>
+      <c r="H24" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="101" t="s">
+      <c r="I24" s="84" t="s">
         <v>615</v>
       </c>
-      <c r="J24" s="100"/>
+      <c r="J24" s="83"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="84" t="s">
         <v>616</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="84" t="s">
         <v>617</v>
       </c>
-      <c r="E25" s="101" t="s">
+      <c r="E25" s="84" t="s">
         <v>528</v>
       </c>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="101" t="s">
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="I25" s="101" t="s">
+      <c r="I25" s="84" t="s">
         <v>618</v>
       </c>
-      <c r="J25" s="100"/>
+      <c r="J25" s="83"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="101" t="s">
+      <c r="C26" s="84" t="s">
         <v>619</v>
       </c>
-      <c r="D26" s="101" t="s">
+      <c r="D26" s="84" t="s">
         <v>620</v>
       </c>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="84" t="s">
         <v>621</v>
       </c>
-      <c r="F26" s="101" t="s">
+      <c r="F26" s="84" t="s">
         <v>603</v>
       </c>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101" t="s">
+      <c r="G26" s="84"/>
+      <c r="H26" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="101" t="s">
+      <c r="I26" s="84" t="s">
         <v>622</v>
       </c>
-      <c r="J26" s="100"/>
+      <c r="J26" s="83"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="101" t="s">
+      <c r="C27" s="84" t="s">
         <v>623</v>
       </c>
-      <c r="D27" s="101" t="s">
+      <c r="D27" s="84" t="s">
         <v>624</v>
       </c>
-      <c r="E27" s="101" t="s">
+      <c r="E27" s="84" t="s">
         <v>625</v>
       </c>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101" t="s">
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="101" t="s">
+      <c r="I27" s="84" t="s">
         <v>626</v>
       </c>
-      <c r="J27" s="100"/>
+      <c r="J27" s="83"/>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="101" t="s">
+      <c r="C28" s="84" t="s">
         <v>627</v>
       </c>
-      <c r="D28" s="101" t="s">
+      <c r="D28" s="84" t="s">
         <v>628</v>
       </c>
-      <c r="E28" s="101" t="s">
+      <c r="E28" s="84" t="s">
         <v>629</v>
       </c>
-      <c r="F28" s="101" t="s">
+      <c r="F28" s="84" t="s">
         <v>630</v>
       </c>
-      <c r="G28" s="101" t="s">
+      <c r="G28" s="84" t="s">
         <v>547</v>
       </c>
-      <c r="H28" s="101" t="s">
+      <c r="H28" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="101" t="s">
+      <c r="I28" s="84" t="s">
         <v>631</v>
       </c>
-      <c r="J28" s="100"/>
+      <c r="J28" s="83"/>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="101" t="s">
+      <c r="C29" s="84" t="s">
         <v>632</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="84" t="s">
         <v>633</v>
       </c>
-      <c r="E29" s="101" t="s">
+      <c r="E29" s="84" t="s">
         <v>578</v>
       </c>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101" t="s">
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="I29" s="101" t="s">
+      <c r="I29" s="84" t="s">
         <v>634</v>
       </c>
-      <c r="J29" s="100"/>
+      <c r="J29" s="83"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="101" t="s">
+      <c r="C30" s="84" t="s">
         <v>635</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="84" t="s">
         <v>636</v>
       </c>
-      <c r="E30" s="101" t="s">
+      <c r="E30" s="84" t="s">
         <v>637</v>
       </c>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101" t="s">
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="I30" s="101" t="s">
+      <c r="I30" s="84" t="s">
         <v>638</v>
       </c>
-      <c r="J30" s="100"/>
+      <c r="J30" s="83"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="101" t="s">
+      <c r="C31" s="84" t="s">
         <v>639</v>
       </c>
-      <c r="D31" s="101" t="s">
+      <c r="D31" s="84" t="s">
         <v>640</v>
       </c>
-      <c r="E31" s="101" t="s">
+      <c r="E31" s="84" t="s">
         <v>641</v>
       </c>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101" t="s">
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84" t="s">
         <v>642</v>
       </c>
-      <c r="I31" s="101" t="s">
+      <c r="I31" s="84" t="s">
         <v>643</v>
       </c>
-      <c r="J31" s="100"/>
+      <c r="J31" s="83"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C32" s="101" t="s">
+      <c r="C32" s="84" t="s">
         <v>644</v>
       </c>
-      <c r="D32" s="101" t="s">
+      <c r="D32" s="84" t="s">
         <v>572</v>
       </c>
-      <c r="E32" s="101" t="s">
+      <c r="E32" s="84" t="s">
         <v>645</v>
       </c>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="101" t="s">
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="I32" s="101" t="s">
+      <c r="I32" s="84" t="s">
         <v>646</v>
       </c>
-      <c r="J32" s="100"/>
+      <c r="J32" s="83"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C33" s="101" t="s">
+      <c r="C33" s="84" t="s">
         <v>647</v>
       </c>
-      <c r="D33" s="101" t="s">
+      <c r="D33" s="84" t="s">
         <v>648</v>
       </c>
-      <c r="E33" s="101" t="s">
+      <c r="E33" s="84" t="s">
         <v>649</v>
       </c>
-      <c r="F33" s="101" t="s">
+      <c r="F33" s="84" t="s">
         <v>650</v>
       </c>
-      <c r="G33" s="101"/>
-      <c r="H33" s="101" t="s">
+      <c r="G33" s="84"/>
+      <c r="H33" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="I33" s="101" t="s">
+      <c r="I33" s="84" t="s">
         <v>651</v>
       </c>
-      <c r="J33" s="100"/>
+      <c r="J33" s="83"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="101" t="s">
+      <c r="C34" s="84" t="s">
         <v>652</v>
       </c>
-      <c r="D34" s="101" t="s">
+      <c r="D34" s="84" t="s">
         <v>653</v>
       </c>
-      <c r="E34" s="101" t="s">
+      <c r="E34" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="F34" s="101" t="s">
+      <c r="F34" s="84" t="s">
         <v>655</v>
       </c>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101" t="s">
+      <c r="G34" s="84"/>
+      <c r="H34" s="84" t="s">
         <v>656</v>
       </c>
-      <c r="I34" s="101" t="s">
+      <c r="I34" s="84" t="s">
         <v>657</v>
       </c>
-      <c r="J34" s="100"/>
+      <c r="J34" s="83"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C35" s="101" t="s">
+      <c r="C35" s="84" t="s">
         <v>658</v>
       </c>
-      <c r="D35" s="101" t="s">
+      <c r="D35" s="84" t="s">
         <v>545</v>
       </c>
-      <c r="E35" s="101" t="s">
+      <c r="E35" s="84" t="s">
         <v>659</v>
       </c>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="101" t="s">
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="84" t="s">
         <v>660</v>
       </c>
-      <c r="I35" s="101" t="s">
+      <c r="I35" s="84" t="s">
         <v>661</v>
       </c>
-      <c r="J35" s="100"/>
+      <c r="J35" s="83"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C36" s="101" t="s">
+      <c r="C36" s="84" t="s">
         <v>662</v>
       </c>
-      <c r="D36" s="101" t="s">
+      <c r="D36" s="84" t="s">
         <v>572</v>
       </c>
-      <c r="E36" s="101" t="s">
+      <c r="E36" s="84" t="s">
         <v>604</v>
       </c>
-      <c r="F36" s="101" t="s">
+      <c r="F36" s="84" t="s">
         <v>621</v>
       </c>
-      <c r="G36" s="101"/>
-      <c r="H36" s="101" t="s">
+      <c r="G36" s="84"/>
+      <c r="H36" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="I36" s="101" t="s">
+      <c r="I36" s="84" t="s">
         <v>663</v>
       </c>
-      <c r="J36" s="100"/>
+      <c r="J36" s="83"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C37" s="101" t="s">
+      <c r="C37" s="84" t="s">
         <v>664</v>
       </c>
-      <c r="D37" s="101" t="s">
+      <c r="D37" s="84" t="s">
         <v>665</v>
       </c>
-      <c r="E37" s="101" t="s">
+      <c r="E37" s="84" t="s">
         <v>666</v>
       </c>
-      <c r="F37" s="101" t="s">
+      <c r="F37" s="84" t="s">
         <v>667</v>
       </c>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101" t="s">
+      <c r="G37" s="84"/>
+      <c r="H37" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="I37" s="101" t="s">
+      <c r="I37" s="84" t="s">
         <v>668</v>
       </c>
-      <c r="J37" s="100"/>
+      <c r="J37" s="83"/>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C38" s="101" t="s">
+      <c r="C38" s="84" t="s">
         <v>669</v>
       </c>
-      <c r="D38" s="101" t="s">
+      <c r="D38" s="84" t="s">
         <v>670</v>
       </c>
-      <c r="E38" s="101" t="s">
+      <c r="E38" s="84" t="s">
         <v>671</v>
       </c>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101" t="s">
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="101" t="s">
+      <c r="I38" s="84" t="s">
         <v>672</v>
       </c>
-      <c r="J38" s="100"/>
+      <c r="J38" s="83"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C39" s="101" t="s">
+      <c r="C39" s="84" t="s">
         <v>673</v>
       </c>
-      <c r="D39" s="101" t="s">
+      <c r="D39" s="84" t="s">
         <v>674</v>
       </c>
-      <c r="E39" s="101" t="s">
+      <c r="E39" s="84" t="s">
         <v>675</v>
       </c>
-      <c r="F39" s="101" t="s">
+      <c r="F39" s="84" t="s">
         <v>590</v>
       </c>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101" t="s">
+      <c r="G39" s="84"/>
+      <c r="H39" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="I39" s="101" t="s">
+      <c r="I39" s="84" t="s">
         <v>676</v>
       </c>
-      <c r="J39" s="100"/>
+      <c r="J39" s="83"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C40" s="101" t="s">
+      <c r="C40" s="84" t="s">
         <v>677</v>
       </c>
-      <c r="D40" s="101" t="s">
+      <c r="D40" s="84" t="s">
         <v>678</v>
       </c>
-      <c r="E40" s="101" t="s">
+      <c r="E40" s="84" t="s">
         <v>679</v>
       </c>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="101" t="s">
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="84" t="s">
         <v>680</v>
       </c>
-      <c r="I40" s="101" t="s">
+      <c r="I40" s="84" t="s">
         <v>681</v>
       </c>
-      <c r="J40" s="100"/>
+      <c r="J40" s="83"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C41" s="101" t="s">
+      <c r="C41" s="84" t="s">
         <v>682</v>
       </c>
-      <c r="D41" s="101" t="s">
+      <c r="D41" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="E41" s="101" t="s">
+      <c r="E41" s="84" t="s">
         <v>666</v>
       </c>
-      <c r="F41" s="101" t="s">
+      <c r="F41" s="84" t="s">
         <v>683</v>
       </c>
-      <c r="G41" s="101"/>
-      <c r="H41" s="101" t="s">
+      <c r="G41" s="84"/>
+      <c r="H41" s="84" t="s">
         <v>680</v>
       </c>
-      <c r="I41" s="101" t="s">
+      <c r="I41" s="84" t="s">
         <v>684</v>
       </c>
-      <c r="J41" s="100"/>
+      <c r="J41" s="83"/>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C42" s="101" t="s">
+      <c r="C42" s="84" t="s">
         <v>685</v>
       </c>
-      <c r="D42" s="101" t="s">
+      <c r="D42" s="84" t="s">
         <v>664</v>
       </c>
-      <c r="E42" s="101" t="s">
+      <c r="E42" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="F42" s="101" t="s">
+      <c r="F42" s="84" t="s">
         <v>604</v>
       </c>
-      <c r="G42" s="101"/>
-      <c r="H42" s="101" t="s">
+      <c r="G42" s="84"/>
+      <c r="H42" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="I42" s="101" t="s">
+      <c r="I42" s="84" t="s">
         <v>686</v>
       </c>
-      <c r="J42" s="100"/>
+      <c r="J42" s="83"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C43" s="101" t="s">
+      <c r="C43" s="84" t="s">
         <v>687</v>
       </c>
-      <c r="D43" s="101" t="s">
+      <c r="D43" s="84" t="s">
         <v>688</v>
       </c>
-      <c r="E43" s="101" t="s">
+      <c r="E43" s="84" t="s">
         <v>611</v>
       </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="101" t="s">
+      <c r="F43" s="84"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="I43" s="101" t="s">
+      <c r="I43" s="84" t="s">
         <v>689</v>
       </c>
-      <c r="J43" s="100"/>
+      <c r="J43" s="83"/>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C44" s="101" t="s">
+      <c r="C44" s="84" t="s">
         <v>690</v>
       </c>
-      <c r="D44" s="101" t="s">
+      <c r="D44" s="84" t="s">
         <v>633</v>
       </c>
-      <c r="E44" s="101" t="s">
+      <c r="E44" s="84" t="s">
         <v>691</v>
       </c>
-      <c r="F44" s="101"/>
-      <c r="G44" s="101"/>
-      <c r="H44" s="101" t="s">
+      <c r="F44" s="84"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="I44" s="101" t="s">
+      <c r="I44" s="84" t="s">
         <v>692</v>
       </c>
-      <c r="J44" s="100"/>
+      <c r="J44" s="83"/>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C45" s="101" t="s">
+      <c r="C45" s="84" t="s">
         <v>693</v>
       </c>
-      <c r="D45" s="101" t="s">
+      <c r="D45" s="84" t="s">
         <v>694</v>
       </c>
-      <c r="E45" s="101" t="s">
+      <c r="E45" s="84" t="s">
         <v>695</v>
       </c>
-      <c r="F45" s="101"/>
-      <c r="G45" s="101"/>
-      <c r="H45" s="101" t="s">
+      <c r="F45" s="84"/>
+      <c r="G45" s="84"/>
+      <c r="H45" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I45" s="101" t="s">
+      <c r="I45" s="84" t="s">
         <v>696</v>
       </c>
-      <c r="J45" s="100"/>
+      <c r="J45" s="83"/>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C46" s="101" t="s">
+      <c r="C46" s="84" t="s">
         <v>697</v>
       </c>
-      <c r="D46" s="101" t="s">
+      <c r="D46" s="84" t="s">
         <v>698</v>
       </c>
-      <c r="E46" s="101" t="s">
+      <c r="E46" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="F46" s="101" t="s">
+      <c r="F46" s="84" t="s">
         <v>528</v>
       </c>
-      <c r="G46" s="101"/>
-      <c r="H46" s="101" t="s">
+      <c r="G46" s="84"/>
+      <c r="H46" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I46" s="101" t="s">
+      <c r="I46" s="84" t="s">
         <v>699</v>
       </c>
-      <c r="J46" s="100"/>
+      <c r="J46" s="83"/>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C47" s="101" t="s">
+      <c r="C47" s="84" t="s">
         <v>700</v>
       </c>
-      <c r="D47" s="101" t="s">
+      <c r="D47" s="84" t="s">
         <v>701</v>
       </c>
-      <c r="E47" s="101" t="s">
+      <c r="E47" s="84" t="s">
         <v>702</v>
       </c>
-      <c r="F47" s="101" t="s">
+      <c r="F47" s="84" t="s">
         <v>590</v>
       </c>
-      <c r="G47" s="101"/>
-      <c r="H47" s="101" t="s">
+      <c r="G47" s="84"/>
+      <c r="H47" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I47" s="101" t="s">
+      <c r="I47" s="84" t="s">
         <v>703</v>
       </c>
-      <c r="J47" s="100"/>
+      <c r="J47" s="83"/>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C48" s="101" t="s">
+      <c r="C48" s="84" t="s">
         <v>704</v>
       </c>
-      <c r="D48" s="101" t="s">
+      <c r="D48" s="84" t="s">
         <v>639</v>
       </c>
-      <c r="E48" s="101" t="s">
+      <c r="E48" s="84" t="s">
         <v>621</v>
       </c>
-      <c r="F48" s="101"/>
-      <c r="G48" s="101"/>
-      <c r="H48" s="101" t="s">
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I48" s="101" t="s">
+      <c r="I48" s="84" t="s">
         <v>705</v>
       </c>
-      <c r="J48" s="100"/>
+      <c r="J48" s="83"/>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="101" t="s">
+      <c r="C49" s="84" t="s">
         <v>706</v>
       </c>
-      <c r="D49" s="101" t="s">
+      <c r="D49" s="84" t="s">
         <v>700</v>
       </c>
-      <c r="E49" s="101" t="s">
+      <c r="E49" s="84" t="s">
         <v>542</v>
       </c>
-      <c r="F49" s="101" t="s">
+      <c r="F49" s="84" t="s">
         <v>581</v>
       </c>
-      <c r="G49" s="101"/>
-      <c r="H49" s="101" t="s">
+      <c r="G49" s="84"/>
+      <c r="H49" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I49" s="101" t="s">
+      <c r="I49" s="84" t="s">
         <v>707</v>
       </c>
-      <c r="J49" s="100"/>
+      <c r="J49" s="83"/>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C50" s="101" t="s">
+      <c r="C50" s="84" t="s">
         <v>708</v>
       </c>
-      <c r="D50" s="101" t="s">
+      <c r="D50" s="84" t="s">
         <v>664</v>
       </c>
-      <c r="E50" s="101" t="s">
+      <c r="E50" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="F50" s="101" t="s">
+      <c r="F50" s="84" t="s">
         <v>709</v>
       </c>
-      <c r="G50" s="101"/>
-      <c r="H50" s="101" t="s">
+      <c r="G50" s="84"/>
+      <c r="H50" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I50" s="101" t="s">
+      <c r="I50" s="84" t="s">
         <v>710</v>
       </c>
-      <c r="J50" s="100"/>
+      <c r="J50" s="83"/>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C51" s="101" t="s">
+      <c r="C51" s="84" t="s">
         <v>711</v>
       </c>
-      <c r="D51" s="101" t="s">
+      <c r="D51" s="84" t="s">
         <v>712</v>
       </c>
-      <c r="E51" s="101" t="s">
+      <c r="E51" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="F51" s="101"/>
-      <c r="G51" s="101"/>
-      <c r="H51" s="101" t="s">
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I51" s="101" t="s">
+      <c r="I51" s="84" t="s">
         <v>713</v>
       </c>
-      <c r="J51" s="100"/>
+      <c r="J51" s="83"/>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C52" s="101" t="s">
+      <c r="C52" s="84" t="s">
         <v>714</v>
       </c>
-      <c r="D52" s="101" t="s">
+      <c r="D52" s="84" t="s">
         <v>715</v>
       </c>
-      <c r="E52" s="101" t="s">
+      <c r="E52" s="84" t="s">
         <v>691</v>
       </c>
-      <c r="F52" s="101" t="s">
+      <c r="F52" s="84" t="s">
         <v>716</v>
       </c>
-      <c r="G52" s="101"/>
-      <c r="H52" s="101" t="s">
+      <c r="G52" s="84"/>
+      <c r="H52" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I52" s="101" t="s">
+      <c r="I52" s="84" t="s">
         <v>717</v>
       </c>
-      <c r="J52" s="100"/>
+      <c r="J52" s="83"/>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C53" s="101" t="s">
+      <c r="C53" s="84" t="s">
         <v>718</v>
       </c>
-      <c r="D53" s="101" t="s">
+      <c r="D53" s="84" t="s">
         <v>719</v>
       </c>
-      <c r="E53" s="101" t="s">
+      <c r="E53" s="84" t="s">
         <v>720</v>
       </c>
-      <c r="F53" s="101" t="s">
+      <c r="F53" s="84" t="s">
         <v>721</v>
       </c>
-      <c r="G53" s="101"/>
-      <c r="H53" s="101" t="s">
+      <c r="G53" s="84"/>
+      <c r="H53" s="84" t="s">
         <v>722</v>
       </c>
-      <c r="I53" s="101" t="s">
+      <c r="I53" s="84" t="s">
         <v>723</v>
       </c>
-      <c r="J53" s="100"/>
+      <c r="J53" s="83"/>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C54" s="101" t="s">
+      <c r="C54" s="84" t="s">
         <v>724</v>
       </c>
-      <c r="D54" s="101" t="s">
+      <c r="D54" s="84" t="s">
         <v>725</v>
       </c>
-      <c r="E54" s="101" t="s">
+      <c r="E54" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="F54" s="101" t="s">
+      <c r="F54" s="84" t="s">
         <v>581</v>
       </c>
-      <c r="G54" s="101"/>
-      <c r="H54" s="101" t="s">
+      <c r="G54" s="84"/>
+      <c r="H54" s="84" t="s">
         <v>122</v>
       </c>
-      <c r="I54" s="101" t="s">
+      <c r="I54" s="84" t="s">
         <v>726</v>
       </c>
-      <c r="J54" s="100"/>
+      <c r="J54" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>